<commit_message>
Added a bunch of stuff, made Observed sunburst
But now, for some reason, the predictive sunburst doesn't match.

Also, the colors are off, because I added another category,
unpredicted, to the observed sunburst. I'll have to figure out what's
wrong with the predicted sunburst protovis stuff, and then add
that unpredicted category, so that the colors will match on my observed
and predicted sunbursts

Also, I added a bunch of figures for transcriptions per recording.
I need to go through those.

Also, a bunch of other stuff.

When I'm not working on the command line, I always forget to
commit regularly!
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
+++ b/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="0" windowWidth="30960" windowHeight="19020" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView minimized="1" xWindow="400" yWindow="0" windowWidth="30960" windowHeight="19020" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Source info" sheetId="2" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="chart for a nice coal dower" sheetId="3" r:id="rId3"/>
     <sheet name="chart for top 21" sheetId="7" r:id="rId4"/>
     <sheet name="chart for top 10" sheetId="8" r:id="rId5"/>
-    <sheet name="chart for top 2" sheetId="9" r:id="rId6"/>
-    <sheet name="transcrip per rec percentDPRCTD" sheetId="5" r:id="rId7"/>
+    <sheet name="Top2" sheetId="10" r:id="rId6"/>
+    <sheet name="chart for top 2" sheetId="9" r:id="rId7"/>
+    <sheet name="transcrip per rec percentDPRCTD" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'transcrip per rec percentDPRCTD'!$A$2:$T$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'transcrip per rec percentDPRCTD'!$A$2:$T$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'transcrips per recordingTALLY'!$A$2:$V$183</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -1061,6 +1062,895 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected Freq Metric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$C$3:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>931028.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.851662E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="2101373048"/>
+        <c:axId val="2101370056"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a nice coal dower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$E$3:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a nice cold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a nigh scold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$G$3:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a nye scold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$H$3:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a nye scold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$I$3:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an aye scold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$J$3:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an eye scold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$K$3:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice coal dower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$L$3:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$M$3:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice cole dower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$N$3:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice kohl dower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$O$3:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice-cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$P$3:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>an ice-cold our</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>an ice cold hour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a nice cold hour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'transcrips per recordingTALLY'!$Q$3:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="250"/>
+        <c:axId val="2101364040"/>
+        <c:axId val="2101367016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2101373048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101370056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2101370056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101373048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2101367016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101364040"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2101364040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101367016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -1176,8 +2066,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2145825496"/>
-        <c:axId val="2145831048"/>
+        <c:axId val="2117327640"/>
+        <c:axId val="2117333192"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -1908,11 +2798,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2145842232"/>
-        <c:axId val="2145836792"/>
+        <c:axId val="2117344376"/>
+        <c:axId val="2117338936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2145825496"/>
+        <c:axId val="2117327640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +2830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145831048"/>
+        <c:crossAx val="2117333192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1948,7 +2838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145831048"/>
+        <c:axId val="2117333192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,12 +2873,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145825496"/>
+        <c:crossAx val="2117327640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145836792"/>
+        <c:axId val="2117338936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2017,12 +2907,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145842232"/>
+        <c:crossAx val="2117344376"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2145842232"/>
+        <c:axId val="2117344376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2031,7 +2921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145836792"/>
+        <c:crossAx val="2117338936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2340,8 +3230,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="9"/>
-        <c:axId val="2144986696"/>
-        <c:axId val="2144989672"/>
+        <c:axId val="2102194968"/>
+        <c:axId val="2102197944"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -2580,11 +3470,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2144996136"/>
-        <c:axId val="2144992856"/>
+        <c:axId val="2102204408"/>
+        <c:axId val="2102201128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144986696"/>
+        <c:axId val="2102194968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +3483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144989672"/>
+        <c:crossAx val="2102197944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2601,7 +3491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144989672"/>
+        <c:axId val="2102197944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,12 +3516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144986696"/>
+        <c:crossAx val="2102194968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144992856"/>
+        <c:axId val="2102201128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,12 +3545,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144996136"/>
+        <c:crossAx val="2102204408"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2144996136"/>
+        <c:axId val="2102204408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2669,7 +3559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144992856"/>
+        <c:crossAx val="2102201128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3305,8 +4195,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2145196424"/>
-        <c:axId val="2145199400"/>
+        <c:axId val="2076569576"/>
+        <c:axId val="2076572552"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -5583,11 +6473,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2145205432"/>
-        <c:axId val="2145202440"/>
+        <c:axId val="2076578584"/>
+        <c:axId val="2076575592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2145196424"/>
+        <c:axId val="2076569576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5596,7 +6486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145199400"/>
+        <c:crossAx val="2076572552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5604,7 +6494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145199400"/>
+        <c:axId val="2076572552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5615,12 +6505,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145196424"/>
+        <c:crossAx val="2076569576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145202440"/>
+        <c:axId val="2076575592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5630,12 +6520,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145205432"/>
+        <c:crossAx val="2076578584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2145205432"/>
+        <c:axId val="2076578584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5644,7 +6534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145202440"/>
+        <c:crossAx val="2076575592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5870,8 +6760,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2145325304"/>
-        <c:axId val="2145328280"/>
+        <c:axId val="2076698920"/>
+        <c:axId val="2076701896"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -8148,11 +9038,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2145334312"/>
-        <c:axId val="2145331320"/>
+        <c:axId val="2076707928"/>
+        <c:axId val="2076704936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2145325304"/>
+        <c:axId val="2076698920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8161,7 +9051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145328280"/>
+        <c:crossAx val="2076701896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8169,7 +9059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145328280"/>
+        <c:axId val="2076701896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8180,12 +9070,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145325304"/>
+        <c:crossAx val="2076698920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145331320"/>
+        <c:axId val="2076704936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8195,12 +9085,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145334312"/>
+        <c:crossAx val="2076707928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2145334312"/>
+        <c:axId val="2076707928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8209,7 +9099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145331320"/>
+        <c:crossAx val="2076704936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8219,6 +9109,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8360,8 +9251,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2144621656"/>
-        <c:axId val="2144618664"/>
+        <c:axId val="2102300904"/>
+        <c:axId val="2102303880"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -9624,11 +10515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2144612648"/>
-        <c:axId val="2144615624"/>
+        <c:axId val="2102309912"/>
+        <c:axId val="2102306920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144621656"/>
+        <c:axId val="2102300904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9637,7 +10528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144618664"/>
+        <c:crossAx val="2102303880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9645,7 +10536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144618664"/>
+        <c:axId val="2102303880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9656,12 +10547,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144621656"/>
+        <c:crossAx val="2102300904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144615624"/>
+        <c:axId val="2102306920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9671,12 +10562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144612648"/>
+        <c:crossAx val="2102309912"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2144612648"/>
+        <c:axId val="2102309912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9685,7 +10576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144615624"/>
+        <c:crossAx val="2102306920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9866,8 +10757,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2144499032"/>
-        <c:axId val="2144493464"/>
+        <c:axId val="2101510616"/>
+        <c:axId val="2101505048"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -11130,11 +12021,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2144482296"/>
-        <c:axId val="2144487720"/>
+        <c:axId val="2101493880"/>
+        <c:axId val="2101499304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144499032"/>
+        <c:axId val="2101510616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11162,7 +12053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144493464"/>
+        <c:crossAx val="2101505048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11170,7 +12061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144493464"/>
+        <c:axId val="2101505048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11205,12 +12096,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144499032"/>
+        <c:crossAx val="2101510616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144487720"/>
+        <c:axId val="2101499304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11239,12 +12130,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144482296"/>
+        <c:crossAx val="2101493880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2144482296"/>
+        <c:axId val="2101493880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11253,7 +12144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144487720"/>
+        <c:crossAx val="2101499304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11292,11 +12183,43 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Observed Transcription</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> distribution over all recorded </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>phrases,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> as compared to expected UNISYN frequency metric</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -11314,6 +12237,21 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="0" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
             <a:ln w="28575">
               <a:solidFill>
                 <a:schemeClr val="tx2"/>
@@ -11321,76 +12259,31 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$C$3:$C$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$C$3:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>931028.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.851662E6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.013781E6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>859307.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>826911.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>899370.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>892949.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11398,18 +12291,18 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2144369688"/>
-        <c:axId val="2144366696"/>
+        <c:axId val="-2142178584"/>
+        <c:axId val="-2141431288"/>
       </c:barChart>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -11428,81 +12321,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$E$3:$E$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11524,81 +12376,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$F$3:$F$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11620,81 +12431,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$G$3:$G$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$G$3:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11716,81 +12486,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$H$3:$H$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$H$3:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11812,81 +12541,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$I$3:$I$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$I$3:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11908,81 +12596,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$J$3:$J$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$J$3:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12004,81 +12651,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$K$3:$K$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$K$3:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12100,81 +12706,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$L$3:$L$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$L$3:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12196,81 +12761,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$M$3:$M$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$M$3:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12292,80 +12816,39 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$N$3:$N$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$N$3:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -12388,81 +12871,41 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:separator>, </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$O$3:$O$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$O$3:$O$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12484,81 +12927,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$P$3:$P$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$P$3:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12580,81 +12982,40 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'transcrips per recordingTALLY'!$B$3:$B$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>an ice cold hour</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>a nice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>in ice cold hour</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>a nice old hour</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>a nice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>an ice cold dower</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>an ice coal dower</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>an ice gold hour</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>an eye scold hour</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'transcrips per recordingTALLY'!$Q$3:$Q$11</c:f>
+              <c:f>'transcrips per recordingTALLY'!$Q$3:$Q$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12669,20 +13030,49 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2144360680"/>
-        <c:axId val="2144363656"/>
+        <c:axId val="-2139129784"/>
+        <c:axId val="-2139118632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144369688"/>
+        <c:axId val="-2142178584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Top Two Transcribed Phrases</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144366696"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2141431288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12690,47 +13080,90 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144366696"/>
+        <c:axId val="-2141431288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Expected Freq</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Metric Values</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144369688"/>
+        <c:crossAx val="-2142178584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144363656"/>
+        <c:axId val="-2139118632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="r"/>
+        <c:axPos val="t"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Observed Transcriptions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144360680"/>
+        <c:crossAx val="-2139129784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2144360680"/>
+        <c:axId val="-2139129784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144363656"/>
+        <c:crossAx val="-2139118632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12747,12 +13180,19 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13026,6 +13466,33 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6272696" cy="8105913"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -13066,10 +13533,10 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26445,8 +26912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="H207" sqref="H207"/>
+    <sheetView showRuler="0" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="R91" sqref="R91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26465,8 +26932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView showRuler="0" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26485,8 +26952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="S92" sqref="S92"/>
+    <sheetView showRuler="0" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Made a db for the COCA freqs. Now, to modify code!
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
+++ b/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="400" yWindow="0" windowWidth="30960" windowHeight="19020" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="5900" yWindow="0" windowWidth="26100" windowHeight="19480" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Source info" sheetId="2" r:id="rId1"/>
@@ -15,8 +15,10 @@
     <sheet name="Top2" sheetId="10" r:id="rId6"/>
     <sheet name="chart for top 2" sheetId="9" r:id="rId7"/>
     <sheet name="transcrip per rec percentDPRCTD" sheetId="5" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sheet1!$A$1:$B$179</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'transcrip per rec percentDPRCTD'!$A$2:$T$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'transcrips per recordingTALLY'!$A$2:$V$183</definedName>
   </definedNames>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="223">
   <si>
     <t>Answer.answer</t>
   </si>
@@ -688,6 +690,18 @@
   <si>
     <t>has more than one transcription on at least one recording</t>
   </si>
+  <si>
+    <t>phrase</t>
+  </si>
+  <si>
+    <t>observed count</t>
+  </si>
+  <si>
+    <t>predicted?</t>
+  </si>
+  <si>
+    <t>sum of unpredicteds:</t>
+  </si>
 </sst>
 </file>
 
@@ -735,8 +749,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -744,9 +762,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1133,8 +1155,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2101373048"/>
-        <c:axId val="2101370056"/>
+        <c:axId val="1856190104"/>
+        <c:axId val="1856193080"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -1851,11 +1873,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2101364040"/>
-        <c:axId val="2101367016"/>
+        <c:axId val="1856199112"/>
+        <c:axId val="1856196120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2101373048"/>
+        <c:axId val="1856190104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,7 +1886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101370056"/>
+        <c:crossAx val="1856193080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1872,7 +1894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101370056"/>
+        <c:axId val="1856193080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,12 +1905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101373048"/>
+        <c:crossAx val="1856190104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2101367016"/>
+        <c:axId val="1856196120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1898,12 +1920,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101364040"/>
+        <c:crossAx val="1856199112"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2101364040"/>
+        <c:axId val="1856199112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101367016"/>
+        <c:crossAx val="1856196120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1922,7 +1944,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2066,8 +2087,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2117327640"/>
-        <c:axId val="2117333192"/>
+        <c:axId val="1834064152"/>
+        <c:axId val="1834058584"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -2798,11 +2819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2117344376"/>
-        <c:axId val="2117338936"/>
+        <c:axId val="1834047416"/>
+        <c:axId val="1834052840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117327640"/>
+        <c:axId val="1834064152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2830,7 +2851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117333192"/>
+        <c:crossAx val="1834058584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2838,7 +2859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117333192"/>
+        <c:axId val="1834058584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2873,12 +2894,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117327640"/>
+        <c:crossAx val="1834064152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2117338936"/>
+        <c:axId val="1834052840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2907,12 +2928,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117344376"/>
+        <c:crossAx val="1834047416"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2117344376"/>
+        <c:axId val="1834047416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,7 +2942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117338936"/>
+        <c:crossAx val="1834052840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3230,8 +3251,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="9"/>
-        <c:axId val="2102194968"/>
-        <c:axId val="2102197944"/>
+        <c:axId val="1854321848"/>
+        <c:axId val="1854324824"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -3470,11 +3491,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2102204408"/>
-        <c:axId val="2102201128"/>
+        <c:axId val="1854331288"/>
+        <c:axId val="1854328008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2102194968"/>
+        <c:axId val="1854321848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3483,7 +3504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102197944"/>
+        <c:crossAx val="1854324824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3491,7 +3512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102197944"/>
+        <c:axId val="1854324824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,12 +3537,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102194968"/>
+        <c:crossAx val="1854321848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102201128"/>
+        <c:axId val="1854328008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3545,12 +3566,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102204408"/>
+        <c:crossAx val="1854331288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2102204408"/>
+        <c:axId val="1854331288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3559,7 +3580,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102201128"/>
+        <c:crossAx val="1854328008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4195,8 +4216,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2076569576"/>
-        <c:axId val="2076572552"/>
+        <c:axId val="1836011816"/>
+        <c:axId val="1836014792"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -6473,11 +6494,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2076578584"/>
-        <c:axId val="2076575592"/>
+        <c:axId val="1836020824"/>
+        <c:axId val="1836017832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076569576"/>
+        <c:axId val="1836011816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6486,7 +6507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076572552"/>
+        <c:crossAx val="1836014792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6494,7 +6515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076572552"/>
+        <c:axId val="1836014792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6505,12 +6526,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076569576"/>
+        <c:crossAx val="1836011816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076575592"/>
+        <c:axId val="1836017832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6520,12 +6541,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076578584"/>
+        <c:crossAx val="1836020824"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2076578584"/>
+        <c:axId val="1836020824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6534,7 +6555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076575592"/>
+        <c:crossAx val="1836017832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6760,8 +6781,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2076698920"/>
-        <c:axId val="2076701896"/>
+        <c:axId val="1835039464"/>
+        <c:axId val="1835036472"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -9038,11 +9059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2076707928"/>
-        <c:axId val="2076704936"/>
+        <c:axId val="1835030456"/>
+        <c:axId val="1835033432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076698920"/>
+        <c:axId val="1835039464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9051,7 +9072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076701896"/>
+        <c:crossAx val="1835036472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9059,7 +9080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076701896"/>
+        <c:axId val="1835036472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9070,12 +9091,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076698920"/>
+        <c:crossAx val="1835039464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076704936"/>
+        <c:axId val="1835033432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9085,12 +9106,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076707928"/>
+        <c:crossAx val="1835030456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2076707928"/>
+        <c:axId val="1835030456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9099,7 +9120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076704936"/>
+        <c:crossAx val="1835033432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9109,7 +9130,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9251,8 +9271,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2102300904"/>
-        <c:axId val="2102303880"/>
+        <c:axId val="1834937176"/>
+        <c:axId val="1834940152"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -10515,11 +10535,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2102309912"/>
-        <c:axId val="2102306920"/>
+        <c:axId val="1834946184"/>
+        <c:axId val="1834943192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2102300904"/>
+        <c:axId val="1834937176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10528,7 +10548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102303880"/>
+        <c:crossAx val="1834940152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10536,7 +10556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102303880"/>
+        <c:axId val="1834940152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10547,12 +10567,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102300904"/>
+        <c:crossAx val="1834937176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102306920"/>
+        <c:axId val="1834943192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10562,12 +10582,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102309912"/>
+        <c:crossAx val="1834946184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2102309912"/>
+        <c:axId val="1834946184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10576,7 +10596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102306920"/>
+        <c:crossAx val="1834943192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10757,8 +10777,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2101510616"/>
-        <c:axId val="2101505048"/>
+        <c:axId val="1854478056"/>
+        <c:axId val="1854483608"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -12021,11 +12041,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2101493880"/>
-        <c:axId val="2101499304"/>
+        <c:axId val="1854494792"/>
+        <c:axId val="1854489352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2101510616"/>
+        <c:axId val="1854478056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12053,7 +12073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101505048"/>
+        <c:crossAx val="1854483608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12061,7 +12081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101505048"/>
+        <c:axId val="1854483608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12096,12 +12116,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101510616"/>
+        <c:crossAx val="1854478056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2101499304"/>
+        <c:axId val="1854489352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12130,12 +12150,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101493880"/>
+        <c:crossAx val="1854494792"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2101493880"/>
+        <c:axId val="1854494792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12144,7 +12164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101499304"/>
+        <c:crossAx val="1854489352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12298,8 +12318,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2142178584"/>
-        <c:axId val="-2141431288"/>
+        <c:axId val="1854621080"/>
+        <c:axId val="1854626664"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -13030,11 +13050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2139129784"/>
-        <c:axId val="-2139118632"/>
+        <c:axId val="1854637848"/>
+        <c:axId val="1854632408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2142178584"/>
+        <c:axId val="1854621080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13072,7 +13092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141431288"/>
+        <c:crossAx val="1854626664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13080,7 +13100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141431288"/>
+        <c:axId val="1854626664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13115,12 +13135,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142178584"/>
+        <c:crossAx val="1854621080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139118632"/>
+        <c:axId val="1854632408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13149,12 +13169,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139129784"/>
+        <c:crossAx val="1854637848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2139129784"/>
+        <c:axId val="1854637848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13163,7 +13183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139118632"/>
+        <c:crossAx val="1854632408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13187,7 +13207,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -13468,7 +13488,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6272696" cy="8105913"/>
+    <xdr:ext cx="6285966" cy="8110924"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14159,8 +14179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V183"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26830,6 +26850,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:T183">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+      <formula>2</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -26839,9 +26862,6 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 C3:C183">
@@ -26932,8 +26952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26952,7 +26972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A92" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A72" workbookViewId="0">
       <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
@@ -39393,4 +39413,2083 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D178"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f>IF(C3&lt;&gt;1,B3,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D13" si="0">IF(C4&lt;&gt;1,B4,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>217</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>IF(C15&lt;&gt;1,B15,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>IF(C17&lt;&gt;1,B17,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f>IF(C18&lt;&gt;1,B18,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>IF(C19&lt;&gt;1,B19,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D27" si="1">IF(C21&lt;&gt;1,B21,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" hidden="1">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D36" si="2">IF(C29&lt;&gt;1,B29,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>63</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:D44" si="3">IF(C38&lt;&gt;1,B38,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46:D52" si="4">IF(C46&lt;&gt;1,B46,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" hidden="1">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" hidden="1">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ref="D55:D60" si="5">IF(C55&lt;&gt;1,B55,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" hidden="1">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:D96" si="6">IF(C62&lt;&gt;1,B62,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76">
+        <v>12</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77">
+        <v>352</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89">
+        <v>18</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>103</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1">
+      <c r="A97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <f t="shared" ref="D98:D104" si="7">IF(C98&lt;&gt;1,B98,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" hidden="1">
+      <c r="A105" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <f t="shared" ref="D106:D135" si="8">IF(C106&lt;&gt;1,B106,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>117</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>122</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>123</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>126</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>127</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>129</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>130</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>133</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>134</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>135</v>
+      </c>
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>136</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>137</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>139</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>140</v>
+      </c>
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>141</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>142</v>
+      </c>
+      <c r="B134">
+        <v>38</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="8"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>143</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" hidden="1">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>145</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <f t="shared" ref="D137:D142" si="9">IF(C137&lt;&gt;1,B137,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>146</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>147</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>148</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>149</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>150</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" hidden="1">
+      <c r="A143" t="s">
+        <v>151</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>152</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <f>IF(C144&lt;&gt;1,B144,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>153</v>
+      </c>
+      <c r="B145">
+        <v>9</v>
+      </c>
+      <c r="D145">
+        <f>IF(C145&lt;&gt;1,B145,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>154</v>
+      </c>
+      <c r="B146">
+        <v>2</v>
+      </c>
+      <c r="D146">
+        <f>IF(C146&lt;&gt;1,B146,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" hidden="1">
+      <c r="A147" t="s">
+        <v>155</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>156</v>
+      </c>
+      <c r="B148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <f>IF(C148&lt;&gt;1,B148,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>157</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <f>IF(C149&lt;&gt;1,B149,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <f>IF(C150&lt;&gt;1,B150,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" hidden="1">
+      <c r="A151" t="s">
+        <v>159</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" hidden="1">
+      <c r="A152" t="s">
+        <v>160</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" hidden="1">
+      <c r="A153" t="s">
+        <v>161</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" hidden="1">
+      <c r="A154" t="s">
+        <v>162</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" hidden="1">
+      <c r="A155" t="s">
+        <v>163</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" hidden="1">
+      <c r="A156" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" hidden="1">
+      <c r="A157" t="s">
+        <v>165</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" hidden="1">
+      <c r="A158" t="s">
+        <v>166</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>167</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <f>IF(C159&lt;&gt;1,B159,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" hidden="1">
+      <c r="A160" t="s">
+        <v>168</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" hidden="1">
+      <c r="A161" t="s">
+        <v>169</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" hidden="1">
+      <c r="A162" t="s">
+        <v>170</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" hidden="1">
+      <c r="A163" t="s">
+        <v>171</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" hidden="1">
+      <c r="A164" t="s">
+        <v>16</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" hidden="1">
+      <c r="A165" t="s">
+        <v>172</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" hidden="1">
+      <c r="A166" t="s">
+        <v>173</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" hidden="1">
+      <c r="A167" t="s">
+        <v>174</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" hidden="1">
+      <c r="A168" t="s">
+        <v>175</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" hidden="1">
+      <c r="A169" t="s">
+        <v>176</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" hidden="1">
+      <c r="A170" t="s">
+        <v>177</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" hidden="1">
+      <c r="A171" t="s">
+        <v>178</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>179</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+      <c r="D172">
+        <f>IF(C172&lt;&gt;1,B172,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>180</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <f>IF(C173&lt;&gt;1,B173,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>181</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <f>IF(C174&lt;&gt;1,B174,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>182</v>
+      </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <f>IF(C175&lt;&gt;1,B175,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>183</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <f>IF(C176&lt;&gt;1,B176,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" hidden="1">
+      <c r="A177" t="s">
+        <v>184</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="C178" t="s">
+        <v>222</v>
+      </c>
+      <c r="D178">
+        <f>SUM(D3:D176)</f>
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B179">
+    <filterColumn colId="1">
+      <filters blank="1">
+        <filter val="1"/>
+        <filter val="10"/>
+        <filter val="12"/>
+        <filter val="13"/>
+        <filter val="18"/>
+        <filter val="2"/>
+        <filter val="217"/>
+        <filter val="3"/>
+        <filter val="352"/>
+        <filter val="38"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="63"/>
+        <filter val="9"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:B184">
+      <sortCondition ref="A1:A184"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:B177">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Redid some transcriptons per recording charts by zeroing out blue bar
for three charts, I had non-zero predictions on charts where it shouldve
   been zero. SO I fixed it.
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
+++ b/MechanicalTurkStuff/TranscriptionsPerRecordingCharts_Global.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="0" windowWidth="26100" windowHeight="19480" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="10080" yWindow="0" windowWidth="26100" windowHeight="19480" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Source info" sheetId="2" r:id="rId1"/>
@@ -1156,8 +1156,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128296216"/>
-        <c:axId val="2128299192"/>
+        <c:axId val="2117900536"/>
+        <c:axId val="2117903512"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -1874,11 +1874,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2128305224"/>
-        <c:axId val="2128302232"/>
+        <c:axId val="2117909544"/>
+        <c:axId val="2117906552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128296216"/>
+        <c:axId val="2117900536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,7 +1887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128299192"/>
+        <c:crossAx val="2117903512"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1895,7 +1895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128299192"/>
+        <c:axId val="2117903512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -1908,13 +1908,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128296216"/>
+        <c:crossAx val="2117900536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128302232"/>
+        <c:axId val="2117906552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -1926,14 +1926,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128305224"/>
+        <c:crossAx val="2117909544"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2128305224"/>
+        <c:axId val="2117909544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +1942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128302232"/>
+        <c:crossAx val="2117906552"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1952,7 +1952,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2010,7 +2009,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2096,8 +2094,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128409528"/>
-        <c:axId val="2128415080"/>
+        <c:axId val="2118014360"/>
+        <c:axId val="2118019912"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -2828,11 +2826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2128426264"/>
-        <c:axId val="2128420824"/>
+        <c:axId val="2118031096"/>
+        <c:axId val="2118025656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128409528"/>
+        <c:axId val="2118014360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2854,13 +2852,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128415080"/>
+        <c:crossAx val="2118019912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2868,7 +2865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128415080"/>
+        <c:axId val="2118019912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2896,19 +2893,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128409528"/>
+        <c:crossAx val="2118014360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128420824"/>
+        <c:axId val="2118025656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,19 +2926,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128426264"/>
+        <c:crossAx val="2118031096"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2128426264"/>
+        <c:axId val="2118031096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128420824"/>
+        <c:crossAx val="2118025656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2961,7 +2956,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3089,8 +3083,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2144378632"/>
-        <c:axId val="2144381608"/>
+        <c:axId val="2117216472"/>
+        <c:axId val="2117213480"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -3729,11 +3723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2144525560"/>
-        <c:axId val="2144376984"/>
+        <c:axId val="2117207464"/>
+        <c:axId val="2117210440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144378632"/>
+        <c:axId val="2117216472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,7 +3736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144381608"/>
+        <c:crossAx val="2117213480"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3750,7 +3744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144381608"/>
+        <c:axId val="2117213480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -3763,13 +3757,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144378632"/>
+        <c:crossAx val="2117216472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144376984"/>
+        <c:axId val="2117210440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -3781,14 +3775,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144525560"/>
+        <c:crossAx val="2117207464"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2144525560"/>
+        <c:axId val="2117207464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3797,7 +3791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144376984"/>
+        <c:crossAx val="2117210440"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3935,8 +3929,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2145385560"/>
-        <c:axId val="-2143382248"/>
+        <c:axId val="2117104648"/>
+        <c:axId val="2117101656"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -4575,11 +4569,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2145371000"/>
-        <c:axId val="-2143379208"/>
+        <c:axId val="2117095640"/>
+        <c:axId val="2117098616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145385560"/>
+        <c:axId val="2117104648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4588,7 +4582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143382248"/>
+        <c:crossAx val="2117101656"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4596,7 +4590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143382248"/>
+        <c:axId val="2117101656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -4609,13 +4603,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145385560"/>
+        <c:crossAx val="2117104648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143379208"/>
+        <c:axId val="2117098616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -4627,14 +4621,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145371000"/>
+        <c:crossAx val="2117095640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2145371000"/>
+        <c:axId val="2117095640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4643,7 +4637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143379208"/>
+        <c:crossAx val="2117098616"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4774,7 +4768,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4789,8 +4783,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2143313640"/>
-        <c:axId val="-2143340568"/>
+        <c:axId val="2136207624"/>
+        <c:axId val="2136210600"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -5429,11 +5423,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2143351656"/>
-        <c:axId val="-2143354648"/>
+        <c:axId val="2136216632"/>
+        <c:axId val="2136213640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143313640"/>
+        <c:axId val="2136207624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5442,7 +5436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143340568"/>
+        <c:crossAx val="2136210600"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5450,7 +5444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143340568"/>
+        <c:axId val="2136210600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -5463,13 +5457,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143313640"/>
+        <c:crossAx val="2136207624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143354648"/>
+        <c:axId val="2136213640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -5481,14 +5475,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143351656"/>
+        <c:crossAx val="2136216632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2143351656"/>
+        <c:axId val="2136216632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5497,7 +5491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143354648"/>
+        <c:crossAx val="2136213640"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5628,7 +5622,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5643,8 +5637,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2139530232"/>
-        <c:axId val="-2139611688"/>
+        <c:axId val="2136320888"/>
+        <c:axId val="2136323864"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -6283,11 +6277,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2139454040"/>
-        <c:axId val="-2135677928"/>
+        <c:axId val="2136329896"/>
+        <c:axId val="2136326904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2139530232"/>
+        <c:axId val="2136320888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6296,7 +6290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139611688"/>
+        <c:crossAx val="2136323864"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6304,7 +6298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139611688"/>
+        <c:axId val="2136323864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -6317,13 +6311,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139530232"/>
+        <c:crossAx val="2136320888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135677928"/>
+        <c:axId val="2136326904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -6335,14 +6329,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139454040"/>
+        <c:crossAx val="2136329896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2139454040"/>
+        <c:axId val="2136329896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6351,7 +6345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135677928"/>
+        <c:crossAx val="2136326904"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6482,7 +6476,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6497,8 +6491,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2143147352"/>
-        <c:axId val="-2143035992"/>
+        <c:axId val="2136433624"/>
+        <c:axId val="2136436600"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -7137,11 +7131,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2142534072"/>
-        <c:axId val="-2142895416"/>
+        <c:axId val="2136442632"/>
+        <c:axId val="2136439640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143147352"/>
+        <c:axId val="2136433624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7150,7 +7144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143035992"/>
+        <c:crossAx val="2136436600"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7158,7 +7152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143035992"/>
+        <c:axId val="2136436600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -7171,13 +7165,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143147352"/>
+        <c:crossAx val="2136433624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142895416"/>
+        <c:axId val="2136439640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -7189,14 +7183,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142534072"/>
+        <c:crossAx val="2136442632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2142534072"/>
+        <c:axId val="2136442632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7205,7 +7199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142895416"/>
+        <c:crossAx val="2136439640"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7351,8 +7345,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2131474760"/>
-        <c:axId val="-2131471784"/>
+        <c:axId val="2136545672"/>
+        <c:axId val="2136548648"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -7991,11 +7985,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2131465752"/>
-        <c:axId val="-2131468744"/>
+        <c:axId val="2136554680"/>
+        <c:axId val="2136551688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131474760"/>
+        <c:axId val="2136545672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8004,7 +7998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131471784"/>
+        <c:crossAx val="2136548648"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8012,7 +8006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131471784"/>
+        <c:axId val="2136548648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -8025,13 +8019,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131474760"/>
+        <c:crossAx val="2136545672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2131468744"/>
+        <c:axId val="2136551688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -8043,14 +8037,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131465752"/>
+        <c:crossAx val="2136554680"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2131465752"/>
+        <c:axId val="2136554680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8059,7 +8053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131468744"/>
+        <c:crossAx val="2136551688"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8205,8 +8199,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2127629032"/>
-        <c:axId val="-2128153720"/>
+        <c:axId val="2136662040"/>
+        <c:axId val="2136665016"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -8845,11 +8839,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="-2128147688"/>
-        <c:axId val="-2128150680"/>
+        <c:axId val="2136671048"/>
+        <c:axId val="2136668056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127629032"/>
+        <c:axId val="2136662040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8858,7 +8852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128153720"/>
+        <c:crossAx val="2136665016"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8866,7 +8860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128153720"/>
+        <c:axId val="2136665016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0E6"/>
@@ -8879,13 +8873,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127629032"/>
+        <c:crossAx val="2136662040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0E6"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128150680"/>
+        <c:axId val="2136668056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.0"/>
@@ -8897,14 +8891,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128147688"/>
+        <c:crossAx val="2136671048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2128147688"/>
+        <c:axId val="2136671048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8913,7 +8907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128150680"/>
+        <c:crossAx val="2136668056"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9117,22 +9111,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -9222,8 +9216,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="9"/>
-        <c:axId val="2128059032"/>
-        <c:axId val="2128062008"/>
+        <c:axId val="2052835848"/>
+        <c:axId val="2052838824"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -9462,11 +9456,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2128068472"/>
-        <c:axId val="2128065192"/>
+        <c:axId val="2052845240"/>
+        <c:axId val="2052841960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128059032"/>
+        <c:axId val="2052835848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9475,7 +9469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128062008"/>
+        <c:crossAx val="2052838824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9483,7 +9477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128062008"/>
+        <c:axId val="2052838824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9508,12 +9502,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128059032"/>
+        <c:crossAx val="2052835848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128065192"/>
+        <c:axId val="2052841960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9537,12 +9531,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128068472"/>
+        <c:crossAx val="2052845240"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2128068472"/>
+        <c:axId val="2052845240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9551,7 +9545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128065192"/>
+        <c:crossAx val="2052841960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9900,22 +9894,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -10115,22 +10109,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -10187,8 +10181,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128863464"/>
-        <c:axId val="2128866440"/>
+        <c:axId val="2119553928"/>
+        <c:axId val="2119556904"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -12465,11 +12459,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2128872472"/>
-        <c:axId val="2128869480"/>
+        <c:axId val="2119562936"/>
+        <c:axId val="2119559944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128863464"/>
+        <c:axId val="2119553928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12478,7 +12472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128866440"/>
+        <c:crossAx val="2119556904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12486,7 +12480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128866440"/>
+        <c:axId val="2119556904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12497,12 +12491,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128863464"/>
+        <c:crossAx val="2119553928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128869480"/>
+        <c:axId val="2119559944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12512,12 +12506,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128872472"/>
+        <c:crossAx val="2119562936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2128872472"/>
+        <c:axId val="2119562936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12526,7 +12520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128869480"/>
+        <c:crossAx val="2119559944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12680,22 +12674,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -12752,8 +12746,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128992808"/>
-        <c:axId val="2128995784"/>
+        <c:axId val="2119683272"/>
+        <c:axId val="2119686248"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -15030,11 +15024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2129001816"/>
-        <c:axId val="2128998824"/>
+        <c:axId val="2119692280"/>
+        <c:axId val="2119689288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128992808"/>
+        <c:axId val="2119683272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15043,7 +15037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128995784"/>
+        <c:crossAx val="2119686248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15051,7 +15045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128995784"/>
+        <c:axId val="2119686248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15062,12 +15056,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128992808"/>
+        <c:crossAx val="2119683272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128998824"/>
+        <c:axId val="2119689288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15077,12 +15071,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129001816"/>
+        <c:crossAx val="2119692280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2129001816"/>
+        <c:axId val="2119692280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15091,7 +15085,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128998824"/>
+        <c:crossAx val="2119689288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15209,22 +15203,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -15242,8 +15236,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2129113368"/>
-        <c:axId val="2129116344"/>
+        <c:axId val="2119803560"/>
+        <c:axId val="2119806536"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -16506,11 +16500,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2129122376"/>
-        <c:axId val="2129119384"/>
+        <c:axId val="2119812568"/>
+        <c:axId val="2119809576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129113368"/>
+        <c:axId val="2119803560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16519,7 +16513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129116344"/>
+        <c:crossAx val="2119806536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16527,7 +16521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129116344"/>
+        <c:axId val="2119806536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16538,12 +16532,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129113368"/>
+        <c:crossAx val="2119803560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2129119384"/>
+        <c:axId val="2119809576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16553,12 +16547,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129122376"/>
+        <c:crossAx val="2119812568"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2129122376"/>
+        <c:axId val="2119812568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16567,7 +16561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129119384"/>
+        <c:crossAx val="2119809576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16577,7 +16571,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16715,22 +16708,22 @@
                   <c:v>7.851662E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.503158E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.013781E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.820004E6</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>859307.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>826911.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>899370.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>892949.0</c:v>
@@ -16748,8 +16741,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2129236296"/>
-        <c:axId val="2129241848"/>
+        <c:axId val="2119926344"/>
+        <c:axId val="2119931896"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -18012,11 +18005,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2129253032"/>
-        <c:axId val="2129247592"/>
+        <c:axId val="2119943080"/>
+        <c:axId val="2119937640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129236296"/>
+        <c:axId val="2119926344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18044,7 +18037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129241848"/>
+        <c:crossAx val="2119931896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18052,7 +18045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129241848"/>
+        <c:axId val="2119931896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18087,12 +18080,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129236296"/>
+        <c:crossAx val="2119926344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2129247592"/>
+        <c:axId val="2119937640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18121,12 +18114,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129253032"/>
+        <c:crossAx val="2119943080"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2129253032"/>
+        <c:axId val="2119943080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18135,7 +18128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129247592"/>
+        <c:crossAx val="2119937640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18289,8 +18282,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128118056"/>
-        <c:axId val="2128123640"/>
+        <c:axId val="2120058520"/>
+        <c:axId val="2120064104"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -19021,11 +19014,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="250"/>
-        <c:axId val="2128134824"/>
-        <c:axId val="2128129384"/>
+        <c:axId val="2120075288"/>
+        <c:axId val="2120069848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128118056"/>
+        <c:axId val="2120058520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19063,7 +19056,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128123640"/>
+        <c:crossAx val="2120064104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19071,7 +19064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128123640"/>
+        <c:axId val="2120064104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19106,12 +19099,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128118056"/>
+        <c:crossAx val="2120058520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128129384"/>
+        <c:axId val="2120069848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19140,12 +19133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128134824"/>
+        <c:crossAx val="2120075288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2128134824"/>
+        <c:axId val="2120075288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19154,7 +19147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128129384"/>
+        <c:crossAx val="2120069848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20379,8 +20372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V183"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20688,7 +20681,7 @@
         <v>142</v>
       </c>
       <c r="C5">
-        <v>5503158</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>38</v>
@@ -20826,7 +20819,7 @@
         <v>46</v>
       </c>
       <c r="C7">
-        <v>7820004</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>63</v>
@@ -20895,7 +20888,7 @@
         <v>86</v>
       </c>
       <c r="C8">
-        <v>859307</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -21033,7 +21026,7 @@
         <v>98</v>
       </c>
       <c r="C10">
-        <v>899370</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>18</v>
@@ -33192,8 +33185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A73" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>